<commit_message>
Fixes for TMT data
</commit_message>
<xml_diff>
--- a/examples/my_TMT_experiment.xlsx
+++ b/examples/my_TMT_experiment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="64">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -81,7 +81,7 @@
     <t xml:space="preserve">Condition</t>
   </si>
   <si>
-    <t xml:space="preserve">Set1</t>
+    <t xml:space="preserve">A</t>
   </si>
   <si>
     <t xml:space="preserve">P</t>
@@ -156,7 +156,7 @@
     <t xml:space="preserve">S8</t>
   </si>
   <si>
-    <t xml:space="preserve">Set2</t>
+    <t xml:space="preserve">B</t>
   </si>
   <si>
     <t xml:space="preserve">P3</t>
@@ -190,6 +190,30 @@
   </si>
   <si>
     <t xml:space="preserve">Fraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file1.raw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file2.raw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file3.raw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file4.raw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file5.raw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file6.raw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file7.raw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file8.raw</t>
   </si>
 </sst>
 </file>
@@ -273,7 +297,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -283,6 +307,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -305,15 +333,15 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -426,15 +454,15 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.84074074074074"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.93703703703704"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -954,16 +982,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,306 +1002,70 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
refactored for v1.1 to use modern R packages (data.table) and massively less disk space when the sector size is large
</commit_message>
<xml_diff>
--- a/examples/my_TMT_experiment.xlsx
+++ b/examples/my_TMT_experiment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="56">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -30,34 +30,10 @@
     <t xml:space="preserve">Kendal.Mintcake@footlights.ac.uk</t>
   </si>
   <si>
-    <t xml:space="preserve">model_fc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">norm_nitt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">norm_nburnin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">norm_nchain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">norm_nsamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">model_nitt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">model_nburnin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">model_nchain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">model_nsamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nworker</t>
+    <t xml:space="preserve">max_spectra_per_peptide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nbatch</t>
   </si>
   <si>
     <t xml:space="preserve">Run</t>
@@ -331,17 +307,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.562962962963"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -357,7 +333,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>1.05</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -365,71 +341,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1" t="n">
         <v>100</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -438,7 +350,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -453,523 +365,523 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.93703703703704"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.562962962963"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>126</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>131</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>126</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="D19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>131</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -984,92 +896,92 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.562962962963"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>